<commit_message>
Fixed issues with production files.
</commit_message>
<xml_diff>
--- a/fixed/10V_regulator/275nm_SU_CULBN2/production/ver_0p1_rev_1/BOM_JLCPCB_275nm_SU_CULBN2.xlsx
+++ b/fixed/10V_regulator/275nm_SU_CULBN2/production/ver_0p1_rev_1/BOM_JLCPCB_275nm_SU_CULBN2.xlsx
@@ -212,7 +212,7 @@
     <t xml:space="preserve">SOT-23-5</t>
   </si>
   <si>
-    <t xml:space="preserve">C460356</t>
+    <t xml:space="preserve">C102618</t>
   </si>
   <si>
     <t xml:space="preserve">LMV321 Operational Amplifier </t>
@@ -461,7 +461,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>